<commit_message>
7 and 9 edited from D drive
</commit_message>
<xml_diff>
--- a/OTHERS/New Microsoft Excel Worksheet.xlsx
+++ b/OTHERS/New Microsoft Excel Worksheet.xlsx
@@ -364,7 +364,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,6 +426,9 @@
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -438,6 +441,9 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>